<commit_message>
run transformer against test set
</commit_message>
<xml_diff>
--- a/data/files/training_statistics_transformer.xlsx
+++ b/data/files/training_statistics_transformer.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="30">
   <si>
     <t>embedding model</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>validation f1 micro</t>
+  </si>
+  <si>
+    <t>test f1 micro</t>
   </si>
   <si>
     <t>comment</t>
@@ -423,20 +426,23 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2"/>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2"/>
     </row>
     <row r="2" ht="24.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3">
@@ -447,19 +453,20 @@
         <v>0.6724</v>
       </c>
       <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" ht="24.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3">
@@ -470,19 +477,20 @@
         <v>0.61</v>
       </c>
       <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" ht="24.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3">
@@ -493,46 +501,48 @@
         <v>0.6065</v>
       </c>
       <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" ht="24.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F5" s="3">
         <v>0.7087</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H5" s="3">
         <v>0.6732</v>
       </c>
       <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="3">
@@ -543,19 +553,20 @@
         <v>0.6724</v>
       </c>
       <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="1">
@@ -565,8 +576,10 @@
       <c r="H7" s="1">
         <v>0.6737</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="5"/>
+      <c r="I7" s="1">
+        <v>0.6628</v>
+      </c>
+      <c r="J7" s="4"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
@@ -583,19 +596,20 @@
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="3">
@@ -605,20 +619,23 @@
       <c r="H8" s="3">
         <v>0.6653</v>
       </c>
-      <c r="I8" s="2"/>
+      <c r="I8" s="3">
+        <v>0.6531</v>
+      </c>
+      <c r="J8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="3">
@@ -629,19 +646,20 @@
         <v>0.5897</v>
       </c>
       <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="3">
@@ -652,19 +670,20 @@
         <v>0.6153</v>
       </c>
       <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="3">
@@ -675,19 +694,20 @@
         <v>0.6697</v>
       </c>
       <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="3">
@@ -697,20 +717,23 @@
       <c r="H12" s="3">
         <v>0.6644</v>
       </c>
-      <c r="I12" s="2"/>
+      <c r="I12" s="3">
+        <v>0.6579</v>
+      </c>
+      <c r="J12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="3">
@@ -721,19 +744,20 @@
         <v>0.6237</v>
       </c>
       <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="3">
@@ -744,19 +768,21 @@
         <v>0.6091</v>
       </c>
       <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" s="2"/>
@@ -768,6 +794,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" s="2"/>
@@ -779,6 +806,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" s="2"/>
@@ -790,6 +818,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" s="2"/>
@@ -801,6 +830,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" s="2"/>
@@ -812,6 +842,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" s="2"/>
@@ -823,6 +854,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Best result on test set = 0.6628
</commit_message>
<xml_diff>
--- a/data/files/training_statistics_transformer.xlsx
+++ b/data/files/training_statistics_transformer.xlsx
@@ -552,7 +552,9 @@
       <c r="H6" s="3">
         <v>0.6724</v>
       </c>
-      <c r="I6" s="2"/>
+      <c r="I6" s="1">
+        <v>0.6628</v>
+      </c>
       <c r="J6" s="2"/>
     </row>
     <row r="7">
@@ -576,8 +578,8 @@
       <c r="H7" s="1">
         <v>0.6737</v>
       </c>
-      <c r="I7" s="1">
-        <v>0.6628</v>
+      <c r="I7" s="3">
+        <v>0.6623</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="5"/>

</xml_diff>